<commit_message>
year to sect and instructor objects
</commit_message>
<xml_diff>
--- a/templates/schedule_template.xlsx
+++ b/templates/schedule_template.xlsx
@@ -13,8 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>CLASS SCHEDULE</t>
   </si>
@@ -56,9 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">SAT </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SUN</t>
   </si>
   <si>
     <t>INSTRUCTORS:  Must submit by the 1st week of the term with course number, office hours, tutoring hours, room and if you see students by appointment only. If Distance Learning Only Instructors, please indicate course titles &amp; any office hours available.</t>
@@ -306,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -315,9 +310,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -343,7 +335,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -355,33 +346,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -411,6 +375,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,7 +700,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -703,77 +708,78 @@
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="3" width="14.5703125"/>
     <col min="4" max="4" width="15.28515625"/>
-    <col min="5" max="7" width="14.5703125"/>
+    <col min="5" max="6" width="14.5703125"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="1025" width="14.140625"/>
+    <col min="9" max="979" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
+    </row>
+    <row r="3" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -791,15 +797,13 @@
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="39"/>
+      <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34">
+      <c r="A7" s="23">
         <v>0.29166666666666669</v>
       </c>
       <c r="B7" s="3"/>
@@ -807,11 +811,11 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35">
+      <c r="A8" s="24">
         <v>0.3125</v>
       </c>
       <c r="B8" s="3"/>
@@ -819,11 +823,11 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="40"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="35">
+      <c r="A9" s="24">
         <v>0.33333333333333331</v>
       </c>
       <c r="B9" s="3"/>
@@ -831,11 +835,11 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="35">
+      <c r="A10" s="24">
         <v>0.35416666666666669</v>
       </c>
       <c r="B10" s="3"/>
@@ -843,11 +847,11 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="35">
+      <c r="A11" s="24">
         <v>0.375</v>
       </c>
       <c r="B11" s="3"/>
@@ -855,11 +859,11 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34">
+      <c r="A12" s="23">
         <v>0.39583333333333398</v>
       </c>
       <c r="B12" s="3"/>
@@ -867,11 +871,11 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35">
+      <c r="A13" s="24">
         <v>0.41666666666666702</v>
       </c>
       <c r="B13" s="3"/>
@@ -879,23 +883,23 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="G13" s="41"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="35">
+      <c r="A14" s="24">
         <v>0.4375</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35">
+      <c r="A15" s="24">
         <v>0.45833333333333398</v>
       </c>
       <c r="B15" s="3"/>
@@ -903,11 +907,11 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="35">
+      <c r="A16" s="24">
         <v>0.47916666666666702</v>
       </c>
       <c r="B16" s="3"/>
@@ -915,11 +919,11 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34">
+      <c r="A17" s="23">
         <v>0.5</v>
       </c>
       <c r="B17" s="3"/>
@@ -927,11 +931,11 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="35">
+      <c r="A18" s="24">
         <v>0.52083333333333304</v>
       </c>
       <c r="B18" s="3"/>
@@ -939,11 +943,11 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="35">
+      <c r="A19" s="24">
         <v>0.54166666666666696</v>
       </c>
       <c r="B19" s="3"/>
@@ -951,23 +955,23 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="G19" s="41"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="35">
+      <c r="A20" s="24">
         <v>0.5625</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="35">
+      <c r="A21" s="24">
         <v>0.58333333333333304</v>
       </c>
       <c r="B21" s="3"/>
@@ -975,11 +979,11 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="41"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34">
+      <c r="A22" s="23">
         <v>0.60416666666666696</v>
       </c>
       <c r="B22" s="3"/>
@@ -987,155 +991,155 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="35">
+      <c r="A23" s="24">
         <v>0.625</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="11"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="G23" s="41"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="35">
+      <c r="A24" s="24">
         <v>0.64583333333333304</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="41"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="35">
+      <c r="A25" s="24">
         <v>0.66666666666666696</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="41"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="35">
+      <c r="A26" s="24">
         <v>0.6875</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="41"/>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="34">
+      <c r="A27" s="23">
         <v>0.70833333333333304</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="41"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35">
+      <c r="A28" s="24">
         <v>0.72916666666666696</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="35">
+      <c r="A29" s="24">
         <v>0.75</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="41"/>
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="35">
+      <c r="A30" s="24">
         <v>0.77083333333333304</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="41"/>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="35">
+      <c r="A31" s="24">
         <v>0.79166666666666696</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="G31" s="41"/>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34">
+      <c r="A32" s="23">
         <v>0.8125</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="G32" s="41"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="35">
+      <c r="A33" s="24">
         <v>0.83333333333333304</v>
       </c>
       <c r="B33" s="3"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="G33" s="41"/>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="35">
+      <c r="A34" s="24">
         <v>0.85416666666666696</v>
       </c>
       <c r="B34" s="3"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="41"/>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="35">
+      <c r="A35" s="24">
         <v>0.875</v>
       </c>
       <c r="B35" s="3"/>
@@ -1143,20 +1147,20 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="G35" s="41"/>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
+      <c r="A36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1168,56 +1172,4 @@
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="6" width="8.5703125"/>
-    <col min="7" max="1025" width="14.140625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="6" width="8.5703125"/>
-    <col min="7" max="1025" width="14.140625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
cut off end times at 9pm. Removed double spaces in names
</commit_message>
<xml_diff>
--- a/templates/schedule_template.xlsx
+++ b/templates/schedule_template.xlsx
@@ -376,38 +376,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -416,6 +386,36 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,7 +700,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -715,30 +715,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37">
         <v>2018</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
@@ -775,7 +775,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="37"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -797,7 +797,7 @@
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="39"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
@@ -811,7 +811,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="40"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -823,7 +823,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="40"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -835,7 +835,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="41"/>
+      <c r="G9" s="31"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="41"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="41"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -871,7 +871,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="41"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -883,7 +883,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="41"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -895,7 +895,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="42"/>
+      <c r="G14" s="32"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -907,7 +907,7 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="41"/>
+      <c r="G15" s="31"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -919,7 +919,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="41"/>
+      <c r="G16" s="31"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -931,7 +931,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="41"/>
+      <c r="G17" s="31"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="41"/>
+      <c r="G18" s="31"/>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -955,7 +955,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="41"/>
+      <c r="G19" s="31"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -967,7 +967,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="41"/>
+      <c r="G20" s="31"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -979,7 +979,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="41"/>
+      <c r="G21" s="31"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -991,7 +991,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="41"/>
+      <c r="G22" s="31"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1003,7 +1003,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="10"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="41"/>
+      <c r="G23" s="31"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1015,7 +1015,7 @@
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="41"/>
+      <c r="G24" s="31"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="41"/>
+      <c r="G25" s="31"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1039,7 +1039,7 @@
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="41"/>
+      <c r="G26" s="31"/>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1051,7 +1051,7 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="41"/>
+      <c r="G27" s="31"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1063,7 +1063,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="41"/>
+      <c r="G28" s="31"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1075,7 +1075,7 @@
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="41"/>
+      <c r="G29" s="31"/>
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1087,7 +1087,7 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="41"/>
+      <c r="G30" s="31"/>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1099,7 +1099,7 @@
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="41"/>
+      <c r="G31" s="31"/>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1111,7 +1111,7 @@
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="41"/>
+      <c r="G32" s="31"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1123,7 +1123,7 @@
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="41"/>
+      <c r="G33" s="31"/>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1135,7 +1135,7 @@
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="41"/>
+      <c r="G34" s="31"/>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1147,20 +1147,20 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="41"/>
+      <c r="G35" s="31"/>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="28"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>